<commit_message>
started the tut and finshed my uml
</commit_message>
<xml_diff>
--- a/Product_backlog.xlsx
+++ b/Product_backlog.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harisqureshi/Desktop/stickJumpForce/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1D35DA-86BB-1E48-ADAD-7338EFFE0198}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -14,9 +20,9 @@
     <sheet name="Sprint 4" sheetId="5" r:id="rId5"/>
     <sheet name="Sprint 5" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -513,7 +519,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -591,15 +597,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -610,6 +607,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,8 +635,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -665,7 +681,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -673,11 +689,33 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -757,8 +795,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-40CD-1743-9298-551210F01EED}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="125712256"/>
         <c:axId val="125731200"/>
       </c:lineChart>
@@ -767,6 +819,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -794,7 +847,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -802,9 +855,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -844,12 +918,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="125731200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -895,7 +971,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -903,9 +979,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -948,6 +1045,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -983,8 +1081,18 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1012,7 +1120,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1020,11 +1128,33 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1100,8 +1230,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C45-4E41-8A8C-4CDAD314EF5E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="125804928"/>
         <c:axId val="125806848"/>
       </c:lineChart>
@@ -1110,6 +1254,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1137,7 +1282,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1145,9 +1290,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1187,12 +1353,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="125806848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1234,7 +1402,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1242,9 +1410,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1287,6 +1476,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1322,8 +1512,18 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1351,7 +1551,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1359,11 +1559,33 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1444,8 +1666,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C6F-AF48-B151-43D429BD06D6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="104458496"/>
         <c:axId val="125751680"/>
       </c:lineChart>
@@ -1454,6 +1690,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1481,7 +1718,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1489,9 +1726,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1531,12 +1789,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="125751680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1578,7 +1838,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1586,9 +1846,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1631,6 +1912,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1666,8 +1948,18 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1695,7 +1987,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1703,11 +1995,33 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1788,8 +2102,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1178-D040-8156-1AEB260753B1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="104644992"/>
         <c:axId val="104646912"/>
       </c:lineChart>
@@ -1798,6 +2126,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1825,7 +2154,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1833,9 +2162,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1875,12 +2225,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="104646912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1922,7 +2274,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1930,9 +2282,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1975,6 +2348,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2010,8 +2384,18 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2039,7 +2423,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2047,11 +2431,33 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2132,8 +2538,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3F18-774F-A342-170B03A00982}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="123955072"/>
         <c:axId val="123973632"/>
       </c:lineChart>
@@ -2142,6 +2562,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2169,7 +2590,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2177,9 +2598,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2219,12 +2661,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="123973632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2266,7 +2710,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2274,9 +2718,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2319,6 +2784,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2354,8 +2820,18 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2383,7 +2859,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2391,11 +2867,33 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2476,8 +2974,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C5C8-8047-B566-1F73CBEC0C97}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="104935424"/>
         <c:axId val="104937344"/>
       </c:lineChart>
@@ -2486,6 +2998,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2513,7 +3026,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2521,9 +3034,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2563,12 +3097,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="104937344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2610,7 +3146,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2618,9 +3154,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2663,6 +3220,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6050,7 +6608,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6085,7 +6649,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6120,7 +6690,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -6157,7 +6733,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -6194,7 +6776,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -6231,7 +6819,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -6506,51 +7100,51 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.5546875" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" customWidth="1"/>
+    <col min="6" max="6" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5" customWidth="1"/>
+    <col min="8" max="8" width="24.5" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="18">
+    <row r="2" spans="1:5" ht="19">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" s="4"/>
@@ -6593,7 +7187,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <f>C8-D9</f>
+        <f t="shared" ref="B9:B14" si="0">C8-D9</f>
         <v>28</v>
       </c>
       <c r="C9">
@@ -6601,7 +7195,7 @@
         <v>28</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="12">
+      <c r="E9" s="9">
         <v>43377</v>
       </c>
     </row>
@@ -6610,15 +7204,15 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <f>C9-D10</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:C14" si="0">C9-D9</f>
+        <f t="shared" ref="C10:C14" si="1">C9-D9</f>
         <v>28</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="12">
+      <c r="E10" s="9">
         <v>43384</v>
       </c>
     </row>
@@ -6627,15 +7221,15 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <f>C10-D11</f>
-        <v>28</v>
-      </c>
-      <c r="C11">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="12">
+      <c r="E11" s="9">
         <v>43398</v>
       </c>
     </row>
@@ -6644,15 +7238,15 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <f>C11-D12</f>
-        <v>28</v>
-      </c>
-      <c r="C12">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="12">
+      <c r="E12" s="9">
         <v>43412</v>
       </c>
     </row>
@@ -6661,15 +7255,15 @@
         <v>7</v>
       </c>
       <c r="B13">
-        <f>C12-D13</f>
-        <v>28</v>
-      </c>
-      <c r="C13">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="12">
+      <c r="E13" s="9">
         <v>43419</v>
       </c>
     </row>
@@ -6678,15 +7272,15 @@
         <v>78</v>
       </c>
       <c r="B14">
-        <f>C13-D14</f>
-        <v>28</v>
-      </c>
-      <c r="C14">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>43437</v>
       </c>
     </row>
@@ -6733,10 +7327,10 @@
       <c r="H20" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="K20" s="8"/>
+      <c r="K20" s="13"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
@@ -6780,17 +7374,17 @@
       <c r="G22" t="s">
         <v>81</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="K22" s="10"/>
+      <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:B48" si="1">B22+1</f>
+        <f t="shared" ref="B23:B48" si="2">B22+1</f>
         <v>3</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -6818,7 +7412,7 @@
         <v>97</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -6846,7 +7440,7 @@
         <v>98</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -6874,7 +7468,7 @@
         <v>99</v>
       </c>
       <c r="B26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -6896,7 +7490,7 @@
         <v>100</v>
       </c>
       <c r="B27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -6912,17 +7506,17 @@
       <c r="G27" t="s">
         <v>82</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="J27" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K27" s="10"/>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -6949,7 +7543,7 @@
         <v>101</v>
       </c>
       <c r="B29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -6977,7 +7571,7 @@
         <v>149</v>
       </c>
       <c r="B30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -7003,7 +7597,7 @@
     <row r="31" spans="1:11">
       <c r="A31" s="1"/>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -7025,7 +7619,7 @@
         <v>108</v>
       </c>
       <c r="B32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -7053,7 +7647,7 @@
         <v>101</v>
       </c>
       <c r="B33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -7081,7 +7675,7 @@
         <v>109</v>
       </c>
       <c r="B34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -7103,7 +7697,7 @@
         <v>102</v>
       </c>
       <c r="B35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -7125,7 +7719,7 @@
         <v>103</v>
       </c>
       <c r="B36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -7145,7 +7739,7 @@
     <row r="37" spans="1:11">
       <c r="A37" s="1"/>
       <c r="B37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -7161,7 +7755,7 @@
         <v>110</v>
       </c>
       <c r="B38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -7183,7 +7777,7 @@
         <v>104</v>
       </c>
       <c r="B39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -7205,7 +7799,7 @@
         <v>105</v>
       </c>
       <c r="B40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -7227,7 +7821,7 @@
         <v>106</v>
       </c>
       <c r="B41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -7247,7 +7841,7 @@
     <row r="42" spans="1:11">
       <c r="A42" s="1"/>
       <c r="B42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -7263,7 +7857,7 @@
         <v>111</v>
       </c>
       <c r="B43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="C43" s="6" t="s">
@@ -7285,7 +7879,7 @@
         <v>107</v>
       </c>
       <c r="B44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -7307,7 +7901,7 @@
         <v>112</v>
       </c>
       <c r="B45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -7327,7 +7921,7 @@
     <row r="46" spans="1:11">
       <c r="A46" s="1"/>
       <c r="B46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -7343,7 +7937,7 @@
         <v>112</v>
       </c>
       <c r="B47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="C47" s="6" t="s">
@@ -7365,7 +7959,7 @@
         <v>113</v>
       </c>
       <c r="B48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -7412,31 +8006,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="11">
+      <c r="B1" s="8">
         <v>1</v>
       </c>
     </row>
@@ -7444,7 +8038,7 @@
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="10">
         <v>43371</v>
       </c>
     </row>
@@ -7452,7 +8046,7 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>43377</v>
       </c>
     </row>
@@ -7460,7 +8054,7 @@
       <c r="A5" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <f>COUNT(A18:A45)</f>
         <v>21</v>
       </c>
@@ -7469,7 +8063,7 @@
       <c r="A6" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>155</v>
       </c>
     </row>
@@ -7477,7 +8071,7 @@
       <c r="A7">
         <v>28</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="8">
         <v>20</v>
       </c>
     </row>
@@ -7485,7 +8079,7 @@
       <c r="A8">
         <v>29</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="8">
         <v>21</v>
       </c>
     </row>
@@ -7493,7 +8087,7 @@
       <c r="A9">
         <v>30</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="8">
         <v>21</v>
       </c>
     </row>
@@ -7501,7 +8095,7 @@
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="8">
         <v>21</v>
       </c>
     </row>
@@ -7509,7 +8103,7 @@
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="8">
         <v>21</v>
       </c>
     </row>
@@ -7517,7 +8111,7 @@
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="8">
         <v>21</v>
       </c>
     </row>
@@ -7525,7 +8119,7 @@
       <c r="A13">
         <v>4</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="8">
         <v>21</v>
       </c>
     </row>
@@ -7548,10 +8142,10 @@
       <c r="F17" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="J17" s="8"/>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
@@ -7587,14 +8181,14 @@
       <c r="E19" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J19" s="10"/>
+      <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <f t="shared" ref="A20:A61" si="0">A19+1</f>
+        <f t="shared" ref="A20:A38" si="0">A19+1</f>
         <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -7607,7 +8201,7 @@
         <v>129</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="I20" t="s">
         <v>22</v>
@@ -7631,7 +8225,7 @@
         <v>131</v>
       </c>
       <c r="E21" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="I21" t="s">
         <v>52</v>
@@ -7699,10 +8293,10 @@
       <c r="E24" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="10"/>
+      <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
@@ -7947,7 +8541,7 @@
         <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -8069,7 +8663,7 @@
       <c r="A86" t="s">
         <v>42</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C86" t="s">
@@ -8086,7 +8680,7 @@
       <c r="A87" t="s">
         <v>44</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C87" t="s">
@@ -8108,7 +8702,7 @@
       <c r="A90" t="s">
         <v>48</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="11" t="s">
         <v>49</v>
       </c>
       <c r="C90" t="s">
@@ -8133,16 +8727,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8274,16 +8868,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8415,16 +9009,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8556,16 +9150,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
updated status in scrum
</commit_message>
<xml_diff>
--- a/Product_backlog.xlsx
+++ b/Product_backlog.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882CABAA-D4E6-4AB9-B9C3-74EF9C32CDF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5064" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5064" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,9 +14,9 @@
     <sheet name="Sprint 4" sheetId="5" r:id="rId5"/>
     <sheet name="Sprint 5" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -522,7 +516,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -645,18 +639,8 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -691,7 +675,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -700,12 +683,10 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -785,31 +766,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-40CD-1743-9298-551210F01EED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="112495616"/>
-        <c:axId val="112501888"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="113343104"/>
+        <c:axId val="113353472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112495616"/>
+        <c:axId val="113343104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -837,7 +809,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -848,7 +819,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -883,19 +853,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112501888"/>
+        <c:crossAx val="113353472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112501888"/>
+        <c:axId val="113353472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -941,7 +909,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -952,7 +919,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -981,7 +947,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112495616"/>
+        <c:crossAx val="113343104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -995,7 +961,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1024,25 +989,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1070,7 +1025,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1079,12 +1034,10 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1160,31 +1113,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8C45-4E41-8A8C-4CDAD314EF5E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="112195456"/>
-        <c:axId val="112664576"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="113300992"/>
+        <c:axId val="113302912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112195456"/>
+        <c:axId val="113300992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1212,7 +1156,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1223,7 +1167,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1258,21 +1201,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112664576"/>
+        <c:crossAx val="113302912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112664576"/>
+        <c:axId val="113302912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22"/>
           <c:min val="0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1314,7 +1255,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1325,7 +1266,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1354,7 +1294,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112195456"/>
+        <c:crossAx val="113300992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -1370,7 +1310,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1399,25 +1338,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1445,7 +1374,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1454,12 +1383,10 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1540,31 +1467,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8C6F-AF48-B151-43D429BD06D6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="112595712"/>
-        <c:axId val="112597632"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="113971584"/>
+        <c:axId val="113973504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112595712"/>
+        <c:axId val="113971584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1592,7 +1510,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1603,7 +1521,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1638,19 +1555,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112597632"/>
+        <c:crossAx val="113973504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112597632"/>
+        <c:axId val="113973504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1692,7 +1607,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1703,7 +1618,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1732,7 +1646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112595712"/>
+        <c:crossAx val="113971584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1746,7 +1660,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1775,25 +1688,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1821,7 +1724,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1830,12 +1732,10 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1916,31 +1816,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1178-D040-8156-1AEB260753B1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="112864640"/>
-        <c:axId val="112879104"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="114048000"/>
+        <c:axId val="114058368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112864640"/>
+        <c:axId val="114048000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1968,7 +1859,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1979,7 +1869,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2014,19 +1903,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112879104"/>
+        <c:crossAx val="114058368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112879104"/>
+        <c:axId val="114058368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2068,7 +1955,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2079,7 +1965,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2108,7 +1993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112864640"/>
+        <c:crossAx val="114048000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2122,7 +2007,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2151,25 +2035,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2197,7 +2071,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2206,12 +2079,10 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2292,31 +2163,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3F18-774F-A342-170B03A00982}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="114104192"/>
-        <c:axId val="114139136"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="115348992"/>
+        <c:axId val="115350912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114104192"/>
+        <c:axId val="115348992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2344,7 +2206,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2355,7 +2216,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2390,19 +2250,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114139136"/>
+        <c:crossAx val="115350912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114139136"/>
+        <c:axId val="115350912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2444,7 +2302,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2455,7 +2312,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2484,7 +2340,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114104192"/>
+        <c:crossAx val="115348992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2498,7 +2354,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2527,25 +2382,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2573,7 +2418,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2582,12 +2426,10 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2668,31 +2510,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C5C8-8047-B566-1F73CBEC0C97}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="114017024"/>
-        <c:axId val="114018944"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="115261824"/>
+        <c:axId val="115263744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114017024"/>
+        <c:axId val="115261824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2720,7 +2553,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2731,7 +2563,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2766,19 +2597,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114018944"/>
+        <c:crossAx val="115263744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114018944"/>
+        <c:axId val="115263744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2820,7 +2649,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2831,7 +2659,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2860,7 +2687,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114017024"/>
+        <c:crossAx val="115261824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2874,7 +2701,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2903,7 +2729,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2929,7 +2755,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2970,7 +2796,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3011,7 +2837,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3054,7 +2880,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3097,7 +2923,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3140,7 +2966,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3418,14 +3244,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K51"/>
   <sheetViews>
     <sheetView topLeftCell="A38" workbookViewId="0">
@@ -4324,11 +4150,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -4479,7 +4305,7 @@
         <v>127</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5049,7 +4875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5190,7 +5016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5331,7 +5157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5472,7 +5298,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
completed section 1-3 of tut
</commit_message>
<xml_diff>
--- a/Product_backlog.xlsx
+++ b/Product_backlog.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harisqureshi/Desktop/stickJumpForce/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CAB88F-A8FA-A242-94CC-775D9C588B4D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8484"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 2" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -521,7 +522,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -665,8 +666,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -701,7 +712,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -710,10 +721,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -799,13 +812,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-40CD-1743-9298-551210F01EED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="144184448"/>
         <c:axId val="144186752"/>
       </c:lineChart>
@@ -814,6 +836,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -841,7 +864,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -852,6 +875,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -891,12 +915,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="144186752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -942,7 +968,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -953,6 +979,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -995,6 +1022,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1030,8 +1058,18 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1059,7 +1097,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1068,10 +1106,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1147,13 +1187,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8C45-4E41-8A8C-4CDAD314EF5E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="143896576"/>
         <c:axId val="143898496"/>
       </c:lineChart>
@@ -1162,6 +1211,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1189,7 +1239,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1200,6 +1250,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1239,6 +1290,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="143898496"/>
@@ -1247,6 +1299,7 @@
           <c:max val="22"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1288,7 +1341,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1299,6 +1352,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1343,6 +1397,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1378,8 +1433,18 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1407,7 +1472,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1416,10 +1481,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1501,13 +1568,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8C45-4E41-8A8C-4CDAD314EF5E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="144267520"/>
         <c:axId val="144281984"/>
       </c:lineChart>
@@ -1516,6 +1592,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1543,7 +1620,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1554,6 +1631,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1593,6 +1671,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="144281984"/>
@@ -1601,6 +1680,7 @@
           <c:max val="22"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1642,7 +1722,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1653,6 +1733,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1697,6 +1778,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1751,7 +1833,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1792,7 +1874,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1833,7 +1915,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2109,34 +2191,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.44140625" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5" customWidth="1"/>
+    <col min="8" max="8" width="24.5" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18">
+    <row r="2" spans="1:4" ht="19">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3002,24 +3084,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3545,7 +3627,7 @@
         <v>141</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3732,24 +3814,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="55.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="55.5" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3895,12 +3977,12 @@
         <v>141</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <f t="shared" ref="A19:A35" si="0">A18+1</f>
+        <f t="shared" ref="A19:A34" si="0">A18+1</f>
         <v>2</v>
       </c>
       <c r="B19" s="13" t="s">

</xml_diff>

<commit_message>
edited sprites and scrum update 10/16
</commit_message>
<xml_diff>
--- a/Product_backlog.xlsx
+++ b/Product_backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5004"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5004" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -796,7 +796,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -901,11 +900,11 @@
           </c:extLst>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133531136"/>
-        <c:axId val="133533696"/>
+        <c:axId val="113739264"/>
+        <c:axId val="113741824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133531136"/>
+        <c:axId val="113739264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,7 +935,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -981,14 +979,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133533696"/>
+        <c:crossAx val="113741824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133533696"/>
+        <c:axId val="113741824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1037,7 +1035,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1076,7 +1073,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133531136"/>
+        <c:crossAx val="113739264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1118,7 +1115,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1249,11 +1246,11 @@
           </c:extLst>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133808512"/>
-        <c:axId val="133810432"/>
+        <c:axId val="114082176"/>
+        <c:axId val="114084096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133808512"/>
+        <c:axId val="114082176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1329,14 +1326,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133810432"/>
+        <c:crossAx val="114084096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133810432"/>
+        <c:axId val="114084096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22"/>
@@ -1422,7 +1419,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133808512"/>
+        <c:crossAx val="114082176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -1466,7 +1463,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1609,11 +1606,11 @@
           </c:extLst>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="136227456"/>
-        <c:axId val="136241920"/>
+        <c:axId val="114272896"/>
+        <c:axId val="114287360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136227456"/>
+        <c:axId val="114272896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1689,14 +1686,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136241920"/>
+        <c:crossAx val="114287360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136241920"/>
+        <c:axId val="114287360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22"/>
@@ -1782,7 +1779,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136227456"/>
+        <c:crossAx val="114272896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -1826,7 +1823,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1999,11 +1996,11 @@
           </c:extLst>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="166671488"/>
-        <c:axId val="166673408"/>
+        <c:axId val="114631808"/>
+        <c:axId val="114633728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166671488"/>
+        <c:axId val="114631808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2079,14 +2076,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166673408"/>
+        <c:crossAx val="114633728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166673408"/>
+        <c:axId val="114633728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -2172,7 +2169,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166671488"/>
+        <c:crossAx val="114631808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -2216,7 +2213,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2242,7 +2239,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2283,7 +2280,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2324,7 +2321,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2365,7 +2362,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2641,7 +2638,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2651,7 +2648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -3561,7 +3558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -4983,8 +4980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
latest pulled and increment 2 updated
</commit_message>
<xml_diff>
--- a/Product_backlog.xlsx
+++ b/Product_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harisqureshi/Desktop/stickJumpForce/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dipti.3QTRUS\Desktop\Classes\IntroSoftwareEngr\stickJumpForce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FC6FAB-A6F7-8345-92C8-A1A76D7B9087}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5D8D42-2443-43B7-A8D2-7BEF8A64C813}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="188">
   <si>
     <t>Product Name:</t>
   </si>
@@ -581,6 +586,30 @@
   </si>
   <si>
     <t>xxxxxxxx</t>
+  </si>
+  <si>
+    <t>Game Controller Requirements</t>
+  </si>
+  <si>
+    <t>Story Line Requirements</t>
+  </si>
+  <si>
+    <t>Audio and Visual Requirements</t>
+  </si>
+  <si>
+    <t>AI requirement</t>
+  </si>
+  <si>
+    <t>5) Software process and UML Diagrams</t>
+  </si>
+  <si>
+    <t>7) Delovery and Schedule</t>
+  </si>
+  <si>
+    <t>6)Assumptions and constraints</t>
+  </si>
+  <si>
+    <t>Finalize and complete every requirements and combine</t>
   </si>
 </sst>
 </file>
@@ -682,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -731,6 +760,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2760,42 +2792,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.5" customWidth="1"/>
-    <col min="8" max="8" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="11" max="11" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="19">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="4"/>
@@ -2950,10 +2982,10 @@
       <c r="H20" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="23" t="s">
+      <c r="J20" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="K20" s="23"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
@@ -3001,10 +3033,10 @@
       <c r="G22" t="s">
         <v>70</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="K22" s="22"/>
+      <c r="K22" s="23"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
@@ -3174,10 +3206,10 @@
       <c r="H28" t="s">
         <v>66</v>
       </c>
-      <c r="J28" s="22" t="s">
+      <c r="J28" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="22"/>
+      <c r="K28" s="23"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
@@ -3674,17 +3706,17 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3803,10 +3835,10 @@
       <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="J17" s="23"/>
+      <c r="J17" s="24"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
@@ -3842,10 +3874,10 @@
       <c r="E19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="J19" s="22"/>
+      <c r="J19" s="23"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
@@ -3998,10 +4030,10 @@
       <c r="E26" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="22" t="s">
+      <c r="I26" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="22"/>
+      <c r="J26" s="23"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
@@ -4400,21 +4432,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17:J17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="55.5" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4447,7 +4479,7 @@
       </c>
       <c r="B5" s="10">
         <f>COUNT(A18:A45)</f>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4549,10 +4581,10 @@
       <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="J17" s="23"/>
+      <c r="J17" s="24"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
@@ -4573,7 +4605,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <f t="shared" ref="A19:A34" si="0">A18+1</f>
+        <f t="shared" ref="A19:A43" si="0">A18+1</f>
         <v>2</v>
       </c>
       <c r="B19" s="13" t="s">
@@ -4588,10 +4620,10 @@
       <c r="E19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="J19" s="22"/>
+      <c r="J19" s="23"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
@@ -4768,10 +4800,10 @@
       <c r="E27" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="J27" s="22"/>
+      <c r="J27" s="23"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28">
@@ -4916,7 +4948,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="22" t="s">
         <v>153</v>
       </c>
       <c r="C34" t="s">
@@ -4925,33 +4957,153 @@
       <c r="D34" t="s">
         <v>155</v>
       </c>
-      <c r="E34" s="16"/>
+      <c r="E34" s="16" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="B35"/>
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" t="s">
+        <v>180</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="B36"/>
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="B37"/>
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="B38" s="13"/>
-      <c r="E38" s="4"/>
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="B39" s="13"/>
-      <c r="E39" s="4"/>
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="B40" s="13"/>
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" t="s">
+        <v>185</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="B41" s="13"/>
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" t="s">
+        <v>186</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="B42" s="13"/>
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" t="s">
+        <v>187</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
       <c r="B43" s="13"/>
@@ -5096,17 +5248,17 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="55.5" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5295,10 +5447,10 @@
       <c r="F22" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="J22" s="23"/>
+      <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
@@ -5330,10 +5482,10 @@
         <v>156</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="J24" s="22"/>
+      <c r="J24" s="23"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25">
@@ -5424,7 +5576,7 @@
       <c r="J28" t="s">
         <v>144</v>
       </c>
-      <c r="K28" s="25" t="s">
+      <c r="K28" s="26" t="s">
         <v>161</v>
       </c>
     </row>
@@ -5449,7 +5601,7 @@
       <c r="J29" t="s">
         <v>145</v>
       </c>
-      <c r="K29" s="25"/>
+      <c r="K29" s="26"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30">
@@ -5504,10 +5656,10 @@
         <v>173</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="I32" s="22" t="s">
+      <c r="I32" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="J32" s="22"/>
+      <c r="J32" s="23"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33">

</xml_diff>

<commit_message>
increment 2 in sprint 3
</commit_message>
<xml_diff>
--- a/Product_backlog.xlsx
+++ b/Product_backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dipti.3QTRUS\Desktop\Classes\IntroSoftwareEngr\stickJumpForce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5D8D42-2443-43B7-A8D2-7BEF8A64C813}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A3E716-E492-41AF-A5CA-E1B42D3B6361}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="187">
   <si>
     <t>Product Name:</t>
   </si>
@@ -571,9 +571,6 @@
   </si>
   <si>
     <t>Complete Level 1 design</t>
-  </si>
-  <si>
-    <t>Complete assigned SRA task</t>
   </si>
   <si>
     <t>xxxxxxxxx</t>
@@ -4432,8 +4429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -4479,7 +4476,7 @@
       </c>
       <c r="B5" s="10">
         <f>COUNT(A18:A45)</f>
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4948,7 +4945,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C34" t="s">
@@ -4957,153 +4954,33 @@
       <c r="D34" t="s">
         <v>155</v>
       </c>
-      <c r="E34" s="16" t="s">
-        <v>42</v>
-      </c>
+      <c r="E34" s="16"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C35" t="s">
-        <v>119</v>
-      </c>
-      <c r="D35" t="s">
-        <v>180</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="B35"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C36" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="B36"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C37" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" t="s">
-        <v>182</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="B37"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" t="s">
-        <v>183</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="B38" s="13"/>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C39" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" t="s">
-        <v>184</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="B39" s="13"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C40" t="s">
-        <v>112</v>
-      </c>
-      <c r="D40" t="s">
-        <v>185</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="B40" s="13"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C41" t="s">
-        <v>117</v>
-      </c>
-      <c r="D41" t="s">
-        <v>186</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="B41" s="13"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C42" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" t="s">
-        <v>187</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="B42" s="13"/>
     </row>
     <row r="43" spans="1:5">
       <c r="B43" s="13"/>
@@ -5244,8 +5121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -5291,8 +5168,8 @@
         <v>143</v>
       </c>
       <c r="B5" s="10">
-        <f>COUNT(A23:A54)-1</f>
-        <v>28</v>
+        <f>COUNT(A23:A41)-1</f>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5666,16 +5543,18 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="22" t="s">
         <v>153</v>
       </c>
       <c r="C33" t="s">
         <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>175</v>
-      </c>
-      <c r="E33" s="4"/>
+        <v>155</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="I33" t="s">
         <v>102</v>
       </c>
@@ -5688,16 +5567,18 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>153</v>
+      <c r="B34" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
-        <v>175</v>
-      </c>
-      <c r="E34" s="4"/>
+        <v>179</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="I34" t="s">
         <v>104</v>
       </c>
@@ -5710,16 +5591,18 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>153</v>
+      <c r="B35" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="C35" t="s">
         <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>175</v>
-      </c>
-      <c r="E35" s="4"/>
+        <v>180</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="I35" t="s">
         <v>106</v>
       </c>
@@ -5732,16 +5615,18 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B36" s="18" t="s">
-        <v>153</v>
+      <c r="B36" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D36" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="4"/>
+        <v>181</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="I36" t="s">
         <v>108</v>
       </c>
@@ -5751,22 +5636,20 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37">
-        <v>0</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>179</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>159</v>
       </c>
       <c r="I37" t="s">
         <v>75</v>
@@ -5777,250 +5660,306 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
-        <v>15</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>163</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="C38" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>165</v>
-      </c>
-      <c r="E38" s="4"/>
+        <v>183</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39">
         <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>164</v>
+        <v>17</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D39" t="s">
-        <v>167</v>
-      </c>
-      <c r="E39" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>163</v>
+        <v>18</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>166</v>
+        <v>185</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41">
         <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>163</v>
+        <v>19</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D41" t="s">
-        <v>166</v>
+        <v>186</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="C42" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" t="s">
-        <v>168</v>
+        <v>0</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f>A43+1</f>
+        <v>16</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="C44" t="s">
         <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f>A44+1</f>
+        <v>17</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="C45" t="s">
         <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <f>A45+1</f>
+        <v>18</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="C46" t="s">
         <v>119</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <f>A46+1</f>
+        <v>19</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="C47" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <f>A47+1</f>
+        <v>20</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>91</v>
+        <v>164</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D48" t="s">
-        <v>61</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <f>A48+1</f>
+        <v>21</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f>A49+1</f>
+        <v>22</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f>A50+1</f>
+        <v>23</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <f>A51+1</f>
+        <v>24</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <f>A52+1</f>
+        <v>25</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <f>A53+1</f>
+        <v>26</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <f>A54+1</f>
+        <v>27</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <f>A55+1</f>
         <v>28</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B56" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C56" t="s">
         <v>117</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D56" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="B52" s="18"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="B53" s="18"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="B54" s="18"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="B55" s="18"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="B56" s="18"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="B57" s="18"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="B58" s="18"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="B59" s="18"/>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="B60" s="18"/>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="B61" s="18"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="B62" s="18"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="B63" s="18"/>
     </row>
     <row r="64" spans="1:4">
       <c r="B64" s="18"/>

</xml_diff>

<commit_message>
completed delivery and schedule in SRA, and updated Scrum
</commit_message>
<xml_diff>
--- a/Product_backlog.xlsx
+++ b/Product_backlog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="184">
   <si>
     <t>Product Name:</t>
   </si>
@@ -567,27 +567,9 @@
     <t>Complete Level 1 design</t>
   </si>
   <si>
-    <t>xxxxxxxxx</t>
-  </si>
-  <si>
-    <t>xxxxxxxxxxx</t>
-  </si>
-  <si>
     <t>COMPLETE UNTIL HERE BY FRIDAY 10/19</t>
   </si>
   <si>
-    <t>xxxxxxxx</t>
-  </si>
-  <si>
-    <t>Game Controller Requirements</t>
-  </si>
-  <si>
-    <t>Story Line Requirements</t>
-  </si>
-  <si>
-    <t>Audio and Visual Requirements</t>
-  </si>
-  <si>
     <t>AI requirement</t>
   </si>
   <si>
@@ -601,6 +583,15 @@
   </si>
   <si>
     <t>Finalize and complete every requirements and combine</t>
+  </si>
+  <si>
+    <t>Menu System Requirements</t>
+  </si>
+  <si>
+    <t>Graphics, and Inventories/Upgrades requirements</t>
+  </si>
+  <si>
+    <t>Character movement requirements</t>
   </si>
 </sst>
 </file>
@@ -658,7 +649,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -689,6 +680,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -702,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -766,6 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,13 +921,12 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="153921792"/>
-        <c:axId val="153923968"/>
+        <c:axId val="46387200"/>
+        <c:axId val="46390656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="153921792"/>
+        <c:axId val="46387200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1004,14 +1001,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153923968"/>
+        <c:crossAx val="46390656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153923968"/>
+        <c:axId val="46390656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,7 +1095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153921792"/>
+        <c:crossAx val="46387200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1140,7 +1137,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1269,13 +1266,12 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="154403968"/>
-        <c:axId val="154405888"/>
+        <c:axId val="107197184"/>
+        <c:axId val="107199104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="154403968"/>
+        <c:axId val="107197184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,14 +1346,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154405888"/>
+        <c:crossAx val="107199104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154405888"/>
+        <c:axId val="107199104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22"/>
@@ -1442,7 +1438,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154403968"/>
+        <c:crossAx val="107197184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -1486,7 +1482,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1627,13 +1623,12 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="154611712"/>
-        <c:axId val="154613632"/>
+        <c:axId val="105457536"/>
+        <c:axId val="105463808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="154611712"/>
+        <c:axId val="105457536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,14 +1703,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154613632"/>
+        <c:crossAx val="105463808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154613632"/>
+        <c:axId val="105463808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22"/>
@@ -1800,7 +1795,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154611712"/>
+        <c:crossAx val="105457536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -1844,7 +1839,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1987,25 +1982,25 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2016,13 +2011,12 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="154372736"/>
-        <c:axId val="154383104"/>
+        <c:axId val="105526016"/>
+        <c:axId val="105527936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="154372736"/>
+        <c:axId val="105526016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,14 +2092,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154383104"/>
+        <c:crossAx val="105527936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154383104"/>
+        <c:axId val="105527936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -2191,7 +2185,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154372736"/>
+        <c:crossAx val="105526016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -2235,7 +2229,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2261,7 +2255,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2302,7 +2296,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2343,7 +2337,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2384,7 +2378,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2660,7 +2654,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5002,8 +4996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -5128,8 +5122,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="10">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -5137,8 +5130,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="10">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -5147,7 +5139,7 @@
       </c>
       <c r="B16" s="10">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -5156,7 +5148,7 @@
       </c>
       <c r="B17" s="10">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -5165,7 +5157,7 @@
       </c>
       <c r="B18" s="10">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -5174,7 +5166,7 @@
       </c>
       <c r="B19" s="10">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -5183,7 +5175,7 @@
       </c>
       <c r="B20" s="10">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -5223,7 +5215,7 @@
       <c r="D23" t="s">
         <v>155</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="27" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5241,7 +5233,7 @@
       <c r="D24" t="s">
         <v>156</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="16"/>
       <c r="I24" s="23" t="s">
         <v>82</v>
       </c>
@@ -5261,8 +5253,8 @@
       <c r="D25" t="s">
         <v>157</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>41</v>
+      <c r="E25" s="27" t="s">
+        <v>42</v>
       </c>
       <c r="I25" t="s">
         <v>20</v>
@@ -5285,7 +5277,7 @@
       <c r="D26" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="16" t="s">
         <v>41</v>
       </c>
       <c r="I26" t="s">
@@ -5309,7 +5301,7 @@
       <c r="D27" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="16"/>
       <c r="I27" t="s">
         <v>42</v>
       </c>
@@ -5331,7 +5323,7 @@
       <c r="D28" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="16"/>
       <c r="I28" s="11"/>
       <c r="J28" t="s">
         <v>144</v>
@@ -5354,7 +5346,7 @@
       <c r="D29" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="16" t="s">
         <v>41</v>
       </c>
       <c r="I29" s="16"/>
@@ -5377,7 +5369,7 @@
       <c r="D30" t="s">
         <v>174</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="16" t="s">
         <v>41</v>
       </c>
       <c r="I30" t="s">
@@ -5401,7 +5393,7 @@
       <c r="D31" t="s">
         <v>172</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="16"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32">
@@ -5417,7 +5409,7 @@
       <c r="D32" t="s">
         <v>173</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="16"/>
       <c r="I32" s="23" t="s">
         <v>11</v>
       </c>
@@ -5427,21 +5419,13 @@
       <c r="A33">
         <v>0</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="19"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>178</v>
-      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="I33" t="s">
         <v>102</v>
       </c>
@@ -5460,11 +5444,9 @@
         <v>119</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>159</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="E34" s="4"/>
       <c r="I34" t="s">
         <v>104</v>
       </c>
@@ -5484,11 +5466,9 @@
         <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>180</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>159</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="E35" s="4"/>
       <c r="I35" t="s">
         <v>106</v>
       </c>
@@ -5510,8 +5490,8 @@
       <c r="D36" t="s">
         <v>181</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>159</v>
+      <c r="E36" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="I36" t="s">
         <v>108</v>
@@ -5532,11 +5512,9 @@
         <v>113</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>159</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="E37" s="4"/>
       <c r="I37" t="s">
         <v>75</v>
       </c>
@@ -5556,11 +5534,9 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>183</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>159</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39">
@@ -5574,10 +5550,10 @@
         <v>112</v>
       </c>
       <c r="D39" t="s">
-        <v>184</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>159</v>
+        <v>178</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -5592,11 +5568,9 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>185</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>159</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41">
@@ -5610,11 +5584,9 @@
         <v>113</v>
       </c>
       <c r="D41" t="s">
-        <v>186</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>159</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42">
@@ -5662,6 +5634,7 @@
       <c r="D44" t="s">
         <v>166</v>
       </c>
+      <c r="E44" s="16"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45">
@@ -5677,6 +5650,7 @@
       <c r="D45" t="s">
         <v>166</v>
       </c>
+      <c r="E45" s="16"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46">
@@ -5692,6 +5666,7 @@
       <c r="D46" t="s">
         <v>168</v>
       </c>
+      <c r="E46" s="16"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47">
@@ -5707,6 +5682,7 @@
       <c r="D47" t="s">
         <v>168</v>
       </c>
+      <c r="E47" s="16"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48">

</xml_diff>